<commit_message>
import multiline adapt basics of configuration
</commit_message>
<xml_diff>
--- a/rmtoo/tests/RMTTest-Import/test-reqs.xlsx
+++ b/rmtoo/tests/RMTTest-Import/test-reqs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="64">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -36,6 +36,9 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Rationale</t>
+  </si>
+  <si>
     <t xml:space="preserve">Status</t>
   </si>
   <si>
@@ -57,9 +60,6 @@
     <t xml:space="preserve">Solved by</t>
   </si>
   <si>
-    <t xml:space="preserve">Rationale</t>
-  </si>
-  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
@@ -78,6 +78,9 @@
     <t xml:space="preserve">\textsl{rmtoo} \textbf{must} support the automatic genration of outputs.</t>
   </si>
   <si>
+    <t xml:space="preserve">Because rmtoo is aimed to be used in productive development environments, there is the need that all the different outputs (e.g. PDFs, graphs, ...) must be generated automatically (without user interaction).</t>
+  </si>
+  <si>
     <t xml:space="preserve">not done</t>
   </si>
   <si>
@@ -96,9 +99,6 @@
     <t xml:space="preserve">Completed</t>
   </si>
   <si>
-    <t xml:space="preserve">Because rmtoo is aimed to be used in productive development environments, there is the need that all the different outputs (e.g. PDFs, graphs, ...) must be generated automatically (without user interaction).</t>
-  </si>
-  <si>
     <t xml:space="preserve">requirement</t>
   </si>
   <si>
@@ -108,13 +108,31 @@
     <t xml:space="preserve">It \textbf{must} be possible to check if a requirement is completed.</t>
   </si>
   <si>
+    <t xml:space="preserve">Completed means that i.e. it and all the children are finished.\par  This can be used for a 'not yet finished' list as an output artifact. </t>
+  </si>
+  <si>
     <t xml:space="preserve">finished</t>
   </si>
   <si>
     <t xml:space="preserve">management:1</t>
   </si>
   <si>
-    <t xml:space="preserve">Completed means that i.e. it and all the children are finished.\par  This can be used for a 'not yet finished' list as an output artifact. </t>
+    <t xml:space="preserve">TestNewlines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Newlines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.
+ASDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.
+QWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lipsum
+Handle it well</t>
   </si>
   <si>
     <t xml:space="preserve">rmtoo</t>
@@ -275,9 +293,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -305,20 +327,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="12" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="15" style="0" width="8.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -332,10 +360,10 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -362,24 +390,24 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -388,58 +416,96 @@
       <c r="G2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="n">
         <v>40221</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="n">
         <v>40243</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>40243</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -471,13 +537,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,72 +551,72 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,53 +624,53 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,34 +678,34 @@
         <v>1</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,26 +713,26 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,15 +740,15 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,170 +764,170 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>